<commit_message>
Packet manager changed to NPM; Admin controllers for editing, creating and deleting added;
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Ads-Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -212,7 +212,7 @@
     <t>Yes - Custom CSS / No responsive design</t>
   </si>
   <si>
-    <t>Very good code separation</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -405,10 +405,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,11 +759,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -781,7 +781,9 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>46</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
       </c>
@@ -819,9 +821,7 @@
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
@@ -1081,15 +1081,15 @@
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
@@ -1099,7 +1099,9 @@
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1109,7 +1111,9 @@
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1119,7 +1123,9 @@
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1129,7 +1135,9 @@
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
@@ -1139,7 +1147,9 @@
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1149,7 +1159,9 @@
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1159,7 +1171,9 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
@@ -1169,7 +1183,9 @@
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
@@ -1179,7 +1195,9 @@
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
@@ -1189,7 +1207,9 @@
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
@@ -1199,7 +1219,9 @@
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
@@ -1209,7 +1231,9 @@
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>
@@ -1219,7 +1243,9 @@
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1255,9 @@
       <c r="B49" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="7"/>
+      <c r="C49" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
@@ -1239,7 +1267,9 @@
       <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D50" s="7" t="s">
         <v>28</v>
       </c>
@@ -1251,7 +1281,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
node_modules added; Self Evaluation edited
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>